<commit_message>
Added the fourth question
</commit_message>
<xml_diff>
--- a/SQL/SQL Questions/SQL_Questions.xlsx
+++ b/SQL/SQL Questions/SQL_Questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mebub_9a7jdi8\Desktop\Important Python Question\SQL\SQL Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E263C6-55E4-4473-B18B-CA51FD1CD603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F0B0E-7A4B-4A60-BFC0-7D40F29E4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2990" windowWidth="14400" windowHeight="7810" xr2:uid="{463E066E-1B96-46FC-B795-0EEAC74A31FE}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>SL.No.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Question</t>
   </si>
@@ -51,16 +48,40 @@
   </si>
   <si>
     <t>Write a query to find the department with the highest total salary paid in the year 2025</t>
+  </si>
+  <si>
+    <t>Q.No.</t>
+  </si>
+  <si>
+    <t>QnA_01</t>
+  </si>
+  <si>
+    <t>QnA_02</t>
+  </si>
+  <si>
+    <t>QnA_03</t>
+  </si>
+  <si>
+    <t>QnA_04</t>
+  </si>
+  <si>
+    <t>Write a query to find the employee with the highest salary in each department in the year 2025.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -422,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9E65EA-A7E7-48FD-B6CA-34CAAAF99A2D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,37 +456,46 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>